<commit_message>
a lot of bug fixes
</commit_message>
<xml_diff>
--- a/carga ejemplo.xlsx
+++ b/carga ejemplo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leox01/Desktop/XXXTREMO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D8659EB-2952-7B4F-B4B4-39A3D4E98980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F0E78D3-8956-4A49-ACE9-BD45C77E44B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{88998EE8-D25E-2243-80CF-FEC39EB7054D}"/>
   </bookViews>
@@ -53,22 +53,22 @@
     <t>Fecha/Hora (opcional)</t>
   </si>
   <si>
-    <t>xlsR1</t>
-  </si>
-  <si>
-    <t>xlsR2</t>
-  </si>
-  <si>
-    <t>xlsR3</t>
-  </si>
-  <si>
-    <t>xlsV1</t>
-  </si>
-  <si>
-    <t>xlsV2</t>
-  </si>
-  <si>
-    <t>xlsV3</t>
+    <t>La Laja</t>
+  </si>
+  <si>
+    <t>Carboneras</t>
+  </si>
+  <si>
+    <t>Cascabeles</t>
+  </si>
+  <si>
+    <t>Jazmin</t>
+  </si>
+  <si>
+    <t>Giro</t>
+  </si>
+  <si>
+    <t>Alonsos</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3">
         <v>100</v>
@@ -508,10 +508,10 @@
     <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3">
         <v>150</v>
@@ -523,7 +523,7 @@
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>

</xml_diff>